<commit_message>
Coloquei mais dados na planilha
</commit_message>
<xml_diff>
--- a/trabalho_peso_3.xlsx
+++ b/trabalho_peso_3.xlsx
@@ -31,8 +31,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -60,9 +68,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B20"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,7 +410,7 @@
         <v>0.02</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:B20" si="0">SIN(A3)</f>
+        <f t="shared" ref="B3:B66" si="0">SIN(A3)</f>
         <v>1.999866669333308E-2</v>
       </c>
     </row>
@@ -556,6 +565,728 @@
       <c r="B20" s="1">
         <f t="shared" si="0"/>
         <v>0.18885889497650057</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.2</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.19866933079506122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.21</v>
+      </c>
+      <c r="B22" s="1">
+        <f t="shared" si="0"/>
+        <v>0.20845989984609956</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.22</v>
+      </c>
+      <c r="B23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.21822962308086932</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.23</v>
+      </c>
+      <c r="B24" s="1">
+        <f t="shared" si="0"/>
+        <v>0.22797752353518841</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.24</v>
+      </c>
+      <c r="B25" s="1">
+        <f t="shared" si="0"/>
+        <v>0.23770262642713458</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.25</v>
+      </c>
+      <c r="B26" s="1">
+        <f t="shared" si="0"/>
+        <v>0.24740395925452294</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0.26</v>
+      </c>
+      <c r="B27" s="1">
+        <f t="shared" si="0"/>
+        <v>0.25708055189215512</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0.27</v>
+      </c>
+      <c r="B28" s="1">
+        <f t="shared" si="0"/>
+        <v>0.26673143668883115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="B29" s="1">
+        <f t="shared" si="0"/>
+        <v>0.27635564856411376</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="B30" s="1">
+        <f t="shared" si="0"/>
+        <v>0.28595222510483553</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0.3</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" si="0"/>
+        <v>0.29552020666133955</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0.31</v>
+      </c>
+      <c r="B32" s="1">
+        <f t="shared" si="0"/>
+        <v>0.3050586364434435</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0.32</v>
+      </c>
+      <c r="B33" s="1">
+        <f t="shared" si="0"/>
+        <v>0.31456656061611776</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>0.33</v>
+      </c>
+      <c r="B34" s="1">
+        <f t="shared" si="0"/>
+        <v>0.32404302839486837</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0.34</v>
+      </c>
+      <c r="B35" s="1">
+        <f t="shared" si="0"/>
+        <v>0.3334870921408144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>0.35</v>
+      </c>
+      <c r="B36" s="1">
+        <f t="shared" si="0"/>
+        <v>0.34289780745545134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>0.36</v>
+      </c>
+      <c r="B37" s="1">
+        <f t="shared" si="0"/>
+        <v>0.35227423327508994</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>0.37</v>
+      </c>
+      <c r="B38" s="1">
+        <f t="shared" si="0"/>
+        <v>0.36161543196496199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>0.38</v>
+      </c>
+      <c r="B39" s="1">
+        <f t="shared" si="0"/>
+        <v>0.37092046941298268</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0.39</v>
+      </c>
+      <c r="B40" s="1">
+        <f t="shared" si="0"/>
+        <v>0.38018841512316143</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0.4</v>
+      </c>
+      <c r="B41" s="1">
+        <f t="shared" si="0"/>
+        <v>0.38941834230865052</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0.41</v>
+      </c>
+      <c r="B42" s="1">
+        <f t="shared" si="0"/>
+        <v>0.39860932798442289</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0.42</v>
+      </c>
+      <c r="B43" s="1">
+        <f t="shared" si="0"/>
+        <v>0.40776045305957015</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>0.43</v>
+      </c>
+      <c r="B44" s="1">
+        <f t="shared" si="0"/>
+        <v>0.41687080242921076</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0.439999999999999</v>
+      </c>
+      <c r="B45" s="1">
+        <f t="shared" si="0"/>
+        <v>0.42593946506599872</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>0.44999999999999901</v>
+      </c>
+      <c r="B46" s="1">
+        <f t="shared" si="0"/>
+        <v>0.43496553411122935</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>0.45999999999999902</v>
+      </c>
+      <c r="B47" s="1">
+        <f t="shared" si="0"/>
+        <v>0.4439481069655189</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>0.46999999999999897</v>
+      </c>
+      <c r="B48" s="1">
+        <f t="shared" si="0"/>
+        <v>0.45288628537906739</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>0.47999999999999898</v>
+      </c>
+      <c r="B49" s="1">
+        <f t="shared" si="0"/>
+        <v>0.46177917554148201</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>0.48999999999999899</v>
+      </c>
+      <c r="B50" s="1">
+        <f t="shared" si="0"/>
+        <v>0.47062588817115714</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>0.499999999999999</v>
+      </c>
+      <c r="B51" s="1">
+        <f t="shared" si="0"/>
+        <v>0.47942553860420212</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>0.50999999999999901</v>
+      </c>
+      <c r="B52" s="1">
+        <f t="shared" si="0"/>
+        <v>0.48817724688290665</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>0.51999999999999902</v>
+      </c>
+      <c r="B53" s="1">
+        <f t="shared" si="0"/>
+        <v>0.49688013784373586</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>0.52999999999999903</v>
+      </c>
+      <c r="B54" s="1">
+        <f t="shared" si="0"/>
+        <v>0.50553334120484616</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>0.53999999999999904</v>
+      </c>
+      <c r="B55" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5141359916531123</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>0.54999999999999905</v>
+      </c>
+      <c r="B56" s="1">
+        <f t="shared" si="0"/>
+        <v>0.52268722893065833</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>0.55999999999999905</v>
+      </c>
+      <c r="B57" s="1">
+        <f t="shared" si="0"/>
+        <v>0.53118619792088262</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>0.56999999999999895</v>
+      </c>
+      <c r="B58" s="1">
+        <f t="shared" si="0"/>
+        <v>0.53963204873396831</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>0.57999999999999896</v>
+      </c>
+      <c r="B59" s="1">
+        <f t="shared" si="0"/>
+        <v>0.54802393679187267</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>0.58999999999999897</v>
+      </c>
+      <c r="B60" s="1">
+        <f t="shared" si="0"/>
+        <v>0.55636102291278289</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>0.59999999999999898</v>
+      </c>
+      <c r="B61" s="1">
+        <f t="shared" si="0"/>
+        <v>0.56464247339503448</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>0.60999999999999899</v>
+      </c>
+      <c r="B62" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5728674601004804</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>0.619999999999999</v>
+      </c>
+      <c r="B63" s="1">
+        <f t="shared" si="0"/>
+        <v>0.58103516053730431</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>0.62999999999999901</v>
+      </c>
+      <c r="B64" s="1">
+        <f t="shared" si="0"/>
+        <v>0.58914475794226873</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>0.63999999999999901</v>
+      </c>
+      <c r="B65" s="1">
+        <f t="shared" si="0"/>
+        <v>0.59719544136239122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>0.64999999999999902</v>
+      </c>
+      <c r="B66" s="1">
+        <f t="shared" si="0"/>
+        <v>0.60518640573603877</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>0.65999999999999903</v>
+      </c>
+      <c r="B67" s="1">
+        <f t="shared" ref="B67:B100" si="1">SIN(A67)</f>
+        <v>0.61311685197343302</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>0.66999999999999904</v>
+      </c>
+      <c r="B68" s="1">
+        <f t="shared" si="1"/>
+        <v>0.62098598703655894</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>0.67999999999999905</v>
+      </c>
+      <c r="B69" s="1">
+        <f t="shared" si="1"/>
+        <v>0.62879302401846782</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>0.68999999999999895</v>
+      </c>
+      <c r="B70" s="1">
+        <f t="shared" si="1"/>
+        <v>0.63653718222196709</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>0.69999999999999896</v>
+      </c>
+      <c r="B71" s="1">
+        <f t="shared" si="1"/>
+        <v>0.64421768723769024</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>0.70999999999999897</v>
+      </c>
+      <c r="B72" s="1">
+        <f t="shared" si="1"/>
+        <v>0.65183377102153595</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>0.71999999999999897</v>
+      </c>
+      <c r="B73" s="1">
+        <f t="shared" si="1"/>
+        <v>0.65938467197147244</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>0.72999999999999898</v>
+      </c>
+      <c r="B74" s="1">
+        <f t="shared" si="1"/>
+        <v>0.66686963500369711</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>0.73999999999999899</v>
+      </c>
+      <c r="B75" s="1">
+        <f t="shared" si="1"/>
+        <v>0.67428791162814428</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>0.749999999999999</v>
+      </c>
+      <c r="B76" s="1">
+        <f t="shared" si="1"/>
+        <v>0.68163876002333346</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>0.75999999999999901</v>
+      </c>
+      <c r="B77" s="1">
+        <f t="shared" si="1"/>
+        <v>0.68892144511055065</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>0.76999999999999902</v>
+      </c>
+      <c r="B78" s="1">
+        <f t="shared" si="1"/>
+        <v>0.69613523862735605</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>0.77999999999999903</v>
+      </c>
+      <c r="B79" s="1">
+        <f t="shared" si="1"/>
+        <v>0.70327941920040948</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>0.78999999999999904</v>
+      </c>
+      <c r="B80" s="1">
+        <f t="shared" si="1"/>
+        <v>0.71035327241760715</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>0.79999999999999905</v>
+      </c>
+      <c r="B81" s="1">
+        <f t="shared" si="1"/>
+        <v>0.71735609089952213</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>0.80999999999999905</v>
+      </c>
+      <c r="B82" s="1">
+        <f t="shared" si="1"/>
+        <v>0.7242871743701419</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>0.81999999999999895</v>
+      </c>
+      <c r="B83" s="1">
+        <f t="shared" si="1"/>
+        <v>0.73114582972689512</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>0.82999999999999896</v>
+      </c>
+      <c r="B84" s="1">
+        <f t="shared" si="1"/>
+        <v>0.73793137110996199</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>0.83999999999999897</v>
+      </c>
+      <c r="B85" s="1">
+        <f t="shared" si="1"/>
+        <v>0.74464311997085864</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>0.84999999999999898</v>
+      </c>
+      <c r="B86" s="1">
+        <f t="shared" si="1"/>
+        <v>0.75128040514029204</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>0.85999999999999899</v>
+      </c>
+      <c r="B87" s="1">
+        <f t="shared" si="1"/>
+        <v>0.75784256289527629</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>0.869999999999999</v>
+      </c>
+      <c r="B88" s="1">
+        <f t="shared" si="1"/>
+        <v>0.76432893702550442</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>0.87999999999999901</v>
+      </c>
+      <c r="B89" s="1">
+        <f t="shared" si="1"/>
+        <v>0.77073887889896864</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>0.88999999999999901</v>
+      </c>
+      <c r="B90" s="1">
+        <f t="shared" si="1"/>
+        <v>0.77707174752682329</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>0.89999999999999902</v>
+      </c>
+      <c r="B91" s="1">
+        <f t="shared" si="1"/>
+        <v>0.78332690962748275</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>0.90999999999999903</v>
+      </c>
+      <c r="B92" s="1">
+        <f t="shared" si="1"/>
+        <v>0.7895037396899498</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>0.91999999999999904</v>
+      </c>
+      <c r="B93" s="1">
+        <f t="shared" si="1"/>
+        <v>0.79560162003636548</v>
+      </c>
+      <c r="D93" s="2"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>0.92999999999999905</v>
+      </c>
+      <c r="B94" s="1">
+        <f t="shared" si="1"/>
+        <v>0.80161994088377664</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>0.93999999999999895</v>
+      </c>
+      <c r="B95" s="1">
+        <f t="shared" si="1"/>
+        <v>0.80755810040511367</v>
+      </c>
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>0.94999999999999796</v>
+      </c>
+      <c r="B96" s="1">
+        <f t="shared" si="1"/>
+        <v>0.81341550478937252</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>0.95999999999999797</v>
+      </c>
+      <c r="B97" s="1">
+        <f t="shared" si="1"/>
+        <v>0.81919156830099715</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>0.96999999999999797</v>
+      </c>
+      <c r="B98" s="1">
+        <f t="shared" si="1"/>
+        <v>0.82488571333844896</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>0.97999999999999798</v>
+      </c>
+      <c r="B99" s="1">
+        <f t="shared" si="1"/>
+        <v>0.83049737049196937</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>0.98999999999999899</v>
+      </c>
+      <c r="B100" s="1">
+        <f t="shared" si="1"/>
+        <v>0.83602597860051997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>